<commit_message>
finished main methods with nutrition functions
</commit_message>
<xml_diff>
--- a/name_method_num_to_method_type.xlsx
+++ b/name_method_num_to_method_type.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chmro\PycharmProjects\GM2-Gibsonify-2022\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B61CE7-3DAB-473C-B4E4-3E506361E20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="18210"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="110">
   <si>
     <t>Method Code</t>
   </si>
@@ -340,12 +346,18 @@
   </si>
   <si>
     <t>BLD+LITTLE-WATER+DRAINED</t>
+  </si>
+  <si>
+    <t>NUTS</t>
+  </si>
+  <si>
+    <t>BOILED+W/DRIPPINGS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -403,6 +415,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -450,7 +465,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -483,9 +498,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,6 +550,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -693,45 +742,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AH21" sqref="AH21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -834,8 +884,11 @@
       <c r="AH1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -938,8 +991,11 @@
       <c r="AH2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1042,8 +1098,11 @@
       <c r="AH3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1146,8 +1205,11 @@
       <c r="AH4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1250,8 +1312,11 @@
       <c r="AH5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1289,7 +1354,7 @@
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1392,8 +1457,11 @@
       <c r="AH7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1496,8 +1564,11 @@
       <c r="AH8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1600,8 +1671,11 @@
       <c r="AH9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1704,8 +1778,11 @@
       <c r="AH10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1743,7 +1820,7 @@
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1781,7 +1858,7 @@
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1878,8 +1955,11 @@
       <c r="AH13" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1917,7 +1997,7 @@
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1955,7 +2035,7 @@
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2058,8 +2138,11 @@
       <c r="AH16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2096,7 +2179,7 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2133,7 +2216,7 @@
       <c r="AH20" s="3"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2170,7 +2253,7 @@
       <c r="AH21" s="3"/>
       <c r="AI21" s="3"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2207,7 +2290,7 @@
       <c r="AH22" s="3"/>
       <c r="AI22" s="3"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2244,7 +2327,7 @@
       <c r="AH23" s="3"/>
       <c r="AI23" s="3"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2281,7 +2364,7 @@
       <c r="AH24" s="3"/>
       <c r="AI24" s="3"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2318,7 +2401,7 @@
       <c r="AH25" s="3"/>
       <c r="AI25" s="3"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2355,7 +2438,7 @@
       <c r="AH26" s="3"/>
       <c r="AI26" s="3"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2392,7 +2475,7 @@
       <c r="AH27" s="3"/>
       <c r="AI27" s="3"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2429,7 +2512,7 @@
       <c r="AH28" s="3"/>
       <c r="AI28" s="3"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2466,7 +2549,7 @@
       <c r="AH29" s="3"/>
       <c r="AI29" s="3"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2503,7 +2586,7 @@
       <c r="AH30" s="3"/>
       <c r="AI30" s="3"/>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2540,7 +2623,7 @@
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2577,7 +2660,7 @@
       <c r="AH32" s="3"/>
       <c r="AI32" s="3"/>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2614,7 +2697,7 @@
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2651,7 +2734,7 @@
       <c r="AH34" s="3"/>
       <c r="AI34" s="3"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2695,24 +2778,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>